<commit_message>
add  two clmn for second foreign and sec en value
</commit_message>
<xml_diff>
--- a/library.xlsx
+++ b/library.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BAC690-CC1E-4FBB-B4F7-1267F2C574ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000C4EFB-2819-4218-90B1-59267546536F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="72">
   <si>
     <t>english</t>
   </si>
@@ -128,6 +128,114 @@
   </si>
   <si>
     <t>ხუთი</t>
+  </si>
+  <si>
+    <t>english_2</t>
+  </si>
+  <si>
+    <t>Hi_2</t>
+  </si>
+  <si>
+    <t>Dog_2</t>
+  </si>
+  <si>
+    <t>Cat_2</t>
+  </si>
+  <si>
+    <t>Lion_2</t>
+  </si>
+  <si>
+    <t>Table_2</t>
+  </si>
+  <si>
+    <t>Pen_2</t>
+  </si>
+  <si>
+    <t>Door_2</t>
+  </si>
+  <si>
+    <t>Apple_2</t>
+  </si>
+  <si>
+    <t>Water_2</t>
+  </si>
+  <si>
+    <t>Red_2</t>
+  </si>
+  <si>
+    <t>Yellow_2</t>
+  </si>
+  <si>
+    <t>Pink_2</t>
+  </si>
+  <si>
+    <t>One_2</t>
+  </si>
+  <si>
+    <t>foreign_2</t>
+  </si>
+  <si>
+    <t>Two_2</t>
+  </si>
+  <si>
+    <t>Three_2</t>
+  </si>
+  <si>
+    <t>Four_2</t>
+  </si>
+  <si>
+    <t>Five_2</t>
+  </si>
+  <si>
+    <t>გამარჯობა_2</t>
+  </si>
+  <si>
+    <t>ძაღლი_2</t>
+  </si>
+  <si>
+    <t>კატა_2</t>
+  </si>
+  <si>
+    <t>ლომი_2</t>
+  </si>
+  <si>
+    <t>მაგიდა_2</t>
+  </si>
+  <si>
+    <t>კალამი_2</t>
+  </si>
+  <si>
+    <t>კარები_2</t>
+  </si>
+  <si>
+    <t>ვაშლი_2</t>
+  </si>
+  <si>
+    <t>წყალი_2</t>
+  </si>
+  <si>
+    <t>წითელი_2</t>
+  </si>
+  <si>
+    <t>ყვითელი_2</t>
+  </si>
+  <si>
+    <t>ვარდისფერი_2</t>
+  </si>
+  <si>
+    <t>ერთი_2</t>
+  </si>
+  <si>
+    <t>ორი_2</t>
+  </si>
+  <si>
+    <t>სამი_2</t>
+  </si>
+  <si>
+    <t>ოთხი_2</t>
+  </si>
+  <si>
+    <t>ხუთი_2</t>
   </si>
 </sst>
 </file>
@@ -448,156 +556,1458 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>39</v>
+      </c>
+      <c r="D55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" t="s">
+        <v>41</v>
+      </c>
+      <c r="D57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" t="s">
+        <v>46</v>
+      </c>
+      <c r="D62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" t="s">
+        <v>51</v>
+      </c>
+      <c r="D66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" t="s">
+        <v>53</v>
+      </c>
+      <c r="D68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" t="s">
+        <v>54</v>
+      </c>
+      <c r="D69" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>37</v>
+      </c>
+      <c r="D70" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s">
+        <v>38</v>
+      </c>
+      <c r="D71" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" t="s">
+        <v>39</v>
+      </c>
+      <c r="D72" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" t="s">
+        <v>23</v>
+      </c>
+      <c r="C74" t="s">
+        <v>41</v>
+      </c>
+      <c r="D74" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D77" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D78" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>15</v>
+      </c>
+      <c r="B79" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79" t="s">
+        <v>46</v>
+      </c>
+      <c r="D79" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" t="s">
+        <v>29</v>
+      </c>
+      <c r="C80" t="s">
+        <v>47</v>
+      </c>
+      <c r="D80" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>17</v>
+      </c>
+      <c r="B81" t="s">
+        <v>30</v>
+      </c>
+      <c r="C81" t="s">
+        <v>48</v>
+      </c>
+      <c r="D81" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" t="s">
+        <v>31</v>
+      </c>
+      <c r="C82" t="s">
+        <v>49</v>
+      </c>
+      <c r="D82" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" t="s">
+        <v>51</v>
+      </c>
+      <c r="D83" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" t="s">
+        <v>52</v>
+      </c>
+      <c r="D84" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" t="s">
+        <v>34</v>
+      </c>
+      <c r="C85" t="s">
+        <v>53</v>
+      </c>
+      <c r="D85" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" t="s">
+        <v>35</v>
+      </c>
+      <c r="C86" t="s">
+        <v>54</v>
+      </c>
+      <c r="D86" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" t="s">
+        <v>37</v>
+      </c>
+      <c r="D87" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>38</v>
+      </c>
+      <c r="D88" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" t="s">
+        <v>39</v>
+      </c>
+      <c r="D89" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" t="s">
+        <v>40</v>
+      </c>
+      <c r="D90" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" t="s">
+        <v>41</v>
+      </c>
+      <c r="D91" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>11</v>
+      </c>
+      <c r="B92" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" t="s">
+        <v>42</v>
+      </c>
+      <c r="D92" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" t="s">
+        <v>25</v>
+      </c>
+      <c r="C93" t="s">
+        <v>43</v>
+      </c>
+      <c r="D93" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>13</v>
+      </c>
+      <c r="B94" t="s">
+        <v>26</v>
+      </c>
+      <c r="C94" t="s">
+        <v>44</v>
+      </c>
+      <c r="D94" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>14</v>
+      </c>
+      <c r="B95" t="s">
+        <v>27</v>
+      </c>
+      <c r="C95" t="s">
+        <v>45</v>
+      </c>
+      <c r="D95" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" t="s">
+        <v>28</v>
+      </c>
+      <c r="C96" t="s">
+        <v>46</v>
+      </c>
+      <c r="D96" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>16</v>
+      </c>
+      <c r="B97" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" t="s">
+        <v>47</v>
+      </c>
+      <c r="D97" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>17</v>
+      </c>
+      <c r="B98" t="s">
+        <v>30</v>
+      </c>
+      <c r="C98" t="s">
+        <v>48</v>
+      </c>
+      <c r="D98" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99" t="s">
+        <v>31</v>
+      </c>
+      <c r="C99" t="s">
+        <v>49</v>
+      </c>
+      <c r="D99" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>19</v>
+      </c>
+      <c r="B100" t="s">
+        <v>32</v>
+      </c>
+      <c r="C100" t="s">
+        <v>51</v>
+      </c>
+      <c r="D100" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s">
+        <v>33</v>
+      </c>
+      <c r="C101" t="s">
+        <v>52</v>
+      </c>
+      <c r="D101" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" t="s">
+        <v>34</v>
+      </c>
+      <c r="C102" t="s">
+        <v>53</v>
+      </c>
+      <c r="D102" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>22</v>
+      </c>
+      <c r="B103" t="s">
+        <v>35</v>
+      </c>
+      <c r="C103" t="s">
+        <v>54</v>
+      </c>
+      <c r="D103" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -633,7 +2043,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C2B8A8B-A809-4727-B1BF-49C96511CDA0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2575AB6-0E27-4C9F-B00A-AB446EED8E74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>